<commit_message>
Issue#17  REQ 3.1   refactor removed invalid test that was broken by jacoco test plugin   test was invalid due to testing scenario that doesn't exist
</commit_message>
<xml_diff>
--- a/broken-file.xlsx
+++ b/broken-file.xlsx
@@ -459,7 +459,7 @@
     <t>e-SRSK</t>
   </si>
   <si>
-    <t>dupa</t>
+    <t>fake</t>
   </si>
 </sst>
 </file>
@@ -1298,7 +1298,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Issue#17  REQ 3.1  RED UNIT TEST for NOT matching correct column order from GOLDEN FILE against  file that was actually read
</commit_message>
<xml_diff>
--- a/broken-file.xlsx
+++ b/broken-file.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Samples" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Samples!$A$1:$K$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Samples!$B$1:$K$28</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="145">
   <si>
     <t>First name</t>
   </si>
@@ -457,9 +457,6 @@
   </si>
   <si>
     <t>e-SRSK</t>
-  </si>
-  <si>
-    <t>fake</t>
   </si>
 </sst>
 </file>
@@ -1295,52 +1292,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" style="4" customWidth="1"/>
     <col min="11" max="11" width="10.5703125" style="4" customWidth="1"/>
     <col min="12" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -1351,34 +1348,31 @@
       <c r="K1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="I2" s="5">
         <v>41764</v>
@@ -1389,34 +1383,31 @@
       <c r="K2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="I3" s="5">
         <v>39295</v>
@@ -1427,28 +1418,25 @@
       <c r="K3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>100</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="I4" s="5">
         <v>39342</v>
@@ -1459,28 +1447,25 @@
       <c r="K4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="I5" s="5">
         <v>39342</v>
@@ -1491,28 +1476,25 @@
       <c r="K5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="I6" s="5">
         <v>39388</v>
@@ -1523,28 +1505,25 @@
       <c r="K6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L6" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="I7" s="5">
         <v>39433</v>
@@ -1555,28 +1534,25 @@
       <c r="K7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L7" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="4" t="s">
@@ -1585,28 +1561,25 @@
       <c r="K8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="L8" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="4" t="s">
@@ -1615,28 +1588,25 @@
       <c r="K9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="L9" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="4" t="s">
@@ -1645,25 +1615,22 @@
       <c r="K10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="L10" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="4" t="s">
@@ -1672,22 +1639,19 @@
       <c r="K11" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="L11" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="4" t="s">
@@ -1696,22 +1660,19 @@
       <c r="K12" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="L12" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="4" t="s">
@@ -1720,22 +1681,19 @@
       <c r="K13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L13" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>141</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>86</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="4" t="s">
@@ -1744,22 +1702,19 @@
       <c r="K14" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="L14" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>142</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="4" t="s">
@@ -1768,22 +1723,19 @@
       <c r="K15" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="L15" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>143</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="4" t="s">
@@ -1792,22 +1744,19 @@
       <c r="K16" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="L16" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>97</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="4" t="s">
@@ -1816,22 +1765,19 @@
       <c r="K17" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="L17" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>98</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="4" t="s">
@@ -1840,22 +1786,19 @@
       <c r="K18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L18" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>99</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="4" t="s">
@@ -1864,22 +1807,19 @@
       <c r="K19" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L19" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>101</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="4" t="s">
@@ -1888,22 +1828,19 @@
       <c r="K20" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="L20" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="E21" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>109</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="4" t="s">
@@ -1912,22 +1849,19 @@
       <c r="K21" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L21" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>111</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="4" t="s">
@@ -1936,22 +1870,19 @@
       <c r="K22" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="L22" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="E23" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="I23" s="5"/>
       <c r="J23" s="4" t="s">
@@ -1960,22 +1891,19 @@
       <c r="K23" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L23" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="E24" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>118</v>
       </c>
       <c r="I24" s="5"/>
       <c r="J24" s="4" t="s">
@@ -1984,22 +1912,19 @@
       <c r="K24" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="L24" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="E25" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>124</v>
       </c>
       <c r="I25" s="5"/>
       <c r="J25" s="4" t="s">
@@ -2008,18 +1933,15 @@
       <c r="K25" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="L25" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B26" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="E26" s="4" t="s">
         <v>74</v>
       </c>
       <c r="I26" s="5"/>
@@ -2029,20 +1951,17 @@
       <c r="K26" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L26" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I28" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K28"/>
-  <sortState ref="F3:F11">
-    <sortCondition ref="F2"/>
+  <autoFilter ref="B1:K28"/>
+  <sortState ref="G3:G11">
+    <sortCondition ref="G2"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>